<commit_message>
update db-benchmark results docs
</commit_message>
<xml_diff>
--- a/20-db-benchmark-results/pivot_exploration.xlsx
+++ b/20-db-benchmark-results/pivot_exploration.xlsx
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="6" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -4518,16 +4518,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>480060</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>914400</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>541020</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8524,7 +8524,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A5:E18" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" showAll="0">
@@ -8935,6 +8935,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="4" tint="0.39997558519241921"/>
+  </sheetPr>
   <dimension ref="A1:A433"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
@@ -11115,10 +11118,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="4" tint="0.39997558519241921"/>
+  </sheetPr>
   <dimension ref="A1:A433"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="A4" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13295,10 +13301,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="4" tint="0.39997558519241921"/>
+  </sheetPr>
   <dimension ref="A1:U433"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A4" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -38299,10 +38308,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="4" tint="0.39997558519241921"/>
+  </sheetPr>
   <dimension ref="A1:G433"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G1048576"/>
+      <selection activeCell="A4" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -48273,18 +48285,22 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="9" tint="0.39997558519241921"/>
+  </sheetPr>
   <dimension ref="A2:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N39" sqref="N39"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26.44140625" customWidth="1"/>
     <col min="2" max="2" width="15.5546875" customWidth="1"/>
-    <col min="3" max="3" width="9" customWidth="1"/>
-    <col min="4" max="6" width="12" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
     <col min="7" max="7" width="12.5546875" customWidth="1"/>
     <col min="8" max="8" width="15.77734375" customWidth="1"/>
     <col min="9" max="9" width="20.44140625" customWidth="1"/>

</xml_diff>